<commit_message>
1 new watershed added but not needed
</commit_message>
<xml_diff>
--- a/selfevaluation.xlsx
+++ b/selfevaluation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Question Number</t>
   </si>
@@ -68,13 +68,16 @@
     <t>Report contains all the neccesary information, pictures, captions and styled.</t>
   </si>
   <si>
-    <t>All the questions are answered by explaining the algorithm's steps but they could have been kept shorter.</t>
-  </si>
-  <si>
-    <t>An actual filtering idea is implemented in a basic way. It's code and before-after pictures are added but it does not find the skin color of the person, instead it uses a constant beige color.</t>
-  </si>
-  <si>
     <t>I have learned a lot by completing this take home and also I have improve my ability to turn an idea into a project.</t>
+  </si>
+  <si>
+    <t>An actual filtering idea implemented in a basic way and added to report. Then the enchanced version is implemented and added to report as well. Before and after pictures along wit Python codes are added.</t>
+  </si>
+  <si>
+    <t>All the questions are answered by explaining the algorithm's steps but they could have been kept even shorter.</t>
+  </si>
+  <si>
+    <t>Explanation No.</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,10 +415,11 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="172.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="188.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,10 +430,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -439,11 +446,14 @@
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -453,11 +463,14 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -465,13 +478,16 @@
         <v>20</v>
       </c>
       <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -479,13 +495,16 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -495,11 +514,14 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -509,11 +531,14 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -521,7 +546,7 @@
         <v>100</v>
       </c>
       <c r="C8">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>